<commit_message>
#Enhancement Version - V1.12
Capture District codes at runtime
Send Email for technical failure
</commit_message>
<xml_diff>
--- a/CowinVaccineAvailabilityProcess/Data/Config.xlsx
+++ b/CowinVaccineAvailabilityProcess/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Uipath\CowinHelpBot\CowinVaccineAvailabilityProcess\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DCC34BD-F4A1-40CE-AF50-E606203948DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4039BC4B-9253-42FE-B3E5-D0830FC41408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -156,6 +156,15 @@
   </si>
   <si>
     <t>CowinGetDistrictEndPoint</t>
+  </si>
+  <si>
+    <t>TechincalFailure</t>
+  </si>
+  <si>
+    <t>Cowin Help Bot Notification - Technical Failure</t>
+  </si>
+  <si>
+    <t>&lt;p style='font-family:Calibri;font-size:11pt'&gt;Hello,&lt;br&gt;&lt;br&gt;The following technical exception occured in Cowin Vaccine Availability Process:#exception. Please go through the orchestrator logs for further details.&lt;br&gt;&lt;br&gt;Regards,&lt;br&gt;Cowin Help Bot&lt;br&gt;UiPath Professional Services-India&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -495,7 +504,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB0D6F91-1792-4E57-8A7C-3F71DC554033}">
   <dimension ref="A1:Z978"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -1719,10 +1728,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X3"/>
+  <dimension ref="A1:X4"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1794,6 +1803,20 @@
         <v>6</v>
       </c>
     </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated Config file and APITracker file
</commit_message>
<xml_diff>
--- a/CowinVaccineAvailabilityProcess/Data/Config.xlsx
+++ b/CowinVaccineAvailabilityProcess/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Uipath\CowinHelpBot\CowinVaccineAvailabilityProcess\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C0FAA1-8F4B-4F9E-B712-5B64438368CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0DF957-D2A1-4CD2-948B-C4C83D15775B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="2" r:id="rId1"/>
@@ -263,9 +263,6 @@
     <t>Cowin Help Bot Notification - Unsubscribed</t>
   </si>
   <si>
-    <t>C:\Users\sukannya.jamadar\OneDrive - UiPath\Desktop\Cowin.xlsx</t>
-  </si>
-  <si>
     <t>VaccineAvailablePincode</t>
   </si>
   <si>
@@ -324,6 +321,9 @@
   </si>
   <si>
     <t>cowin-help@uipath.com</t>
+  </si>
+  <si>
+    <t>C:\UiPath_Files\Cowin.xlsx</t>
   </si>
 </sst>
 </file>
@@ -674,8 +674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB0D6F91-1792-4E57-8A7C-3F71DC554033}">
   <dimension ref="A1:Z980"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -797,7 +797,7 @@
         <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="C10" t="s">
         <v>19</v>
@@ -886,15 +886,15 @@
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" t="s">
         <v>90</v>
-      </c>
-      <c r="B17" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B18">
         <v>5</v>
@@ -902,7 +902,7 @@
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B19">
         <v>100</v>
@@ -910,10 +910,10 @@
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>94</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1890,7 +1890,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58F1AE26-FCFC-41C9-AE03-030E3523569E}">
   <dimension ref="A1:Z9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -2084,13 +2084,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
@@ -2123,13 +2123,13 @@
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:25" ht="43.2" x14ac:dyDescent="0.3">
@@ -2143,13 +2143,13 @@
         <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="86.4" x14ac:dyDescent="0.3">
@@ -2157,19 +2157,19 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="43.2" x14ac:dyDescent="0.3">
@@ -2177,19 +2177,19 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="28.8" x14ac:dyDescent="0.3">
@@ -2203,10 +2203,10 @@
         <v>38</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" t="s">
         <v>84</v>
-      </c>
-      <c r="F6" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="28.8" x14ac:dyDescent="0.3">
@@ -2220,10 +2220,10 @@
         <v>59</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="28.8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Divide and provide information on vaccine capacity based on dose1 or dose2 capacity
#Enhancement - Added two more fields to provide information on vaccine capacity based on dose1 or dose2 capacities
</commit_message>
<xml_diff>
--- a/CowinVaccineAvailabilityProcess/Data/Config.xlsx
+++ b/CowinVaccineAvailabilityProcess/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Uipath\CowinHelpBot\CowinVaccineAvailabilityProcess\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0DF957-D2A1-4CD2-948B-C4C83D15775B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D3E2A9-C2D0-4305-B0B7-646D9E9B3BE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="98">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -56,9 +56,6 @@
     <t>Cowin Help Bot Notification - Vaccination Slots - #District</t>
   </si>
   <si>
-    <t>&lt;p style='font-family:Calibri;font-size:11pt'&gt;Hello,&lt;br&gt;&lt;br&gt;Hope you are safe! &lt;br&gt;&lt;br&gt;Please find below the list of Covid19 vaccination centers available for District : &lt;b&gt;#District&lt;/b&gt; and Age Limit : &lt;b&gt;#AgeLimit.&lt;/b&gt; Please login to &lt;a href="https://www.cowin.gov.in/home"&gt;Cowin Portal&lt;/a&gt; and block your slots immediately.&lt;br&gt;&lt;br&gt;&lt;style&gt;table {font-family: Calibri, sans-serif;font-size:11pt;border-collapse: collapse;width: 100%;}td, th {border: 1px solid #dddddd;text-align: left;padding:8px;}&lt;/style&gt;&lt;table&gt;&lt;tr&gt;&lt;th&gt;Date&lt;/th&gt;&lt;th&gt;Center Name&lt;/th&gt;&lt;th&gt;Center Address&lt;/th&gt;&lt;th&gt;Area&lt;/th&gt;&lt;th&gt;Pincode&lt;/th&gt;&lt;th&gt;Fee Type&lt;/th&gt;&lt;th&gt;Available Capacity&lt;/th&gt;&lt;th&gt;Vaccine Name&lt;/th&gt;&lt;th&gt;Slots Available&lt;/th&gt;&lt;/tr&gt;#DynamicTable&lt;/table&gt;&lt;br&gt;&lt;br&gt;Considering I will be busy monitoring the Cowin site for available vaccine slots, I may not be able to respond to your emails.&lt;br&gt;&lt;br&gt;To unsubscribe, please &lt;a href="#CowinExcel"&gt;click here&lt;/a&gt; and select unsubscribe from the drop down.&lt;br&gt;&lt;br&gt;Regards,&lt;br&gt;Cowin Help Bot&lt;br&gt;UiPath Professional Services-India&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -281,9 +278,6 @@
     <t>#District,#AgeLimit,#CowinExcel</t>
   </si>
   <si>
-    <t>&lt;p style='font-family:Calibri;font-size:11pt'&gt;Hello,&lt;br&gt;&lt;br&gt;Hope you are safe! &lt;br&gt;&lt;br&gt;Please find below the list of Covid19 vaccination centers available for Pincode : &lt;b&gt;#Pincode&lt;/b&gt; and Age Limit : &lt;b&gt;#AgeLimit.&lt;/b&gt; Please login to &lt;a href="https://www.cowin.gov.in/home"&gt;Cowin Portal&lt;/a&gt; and block your slots immediately.&lt;br&gt;&lt;br&gt;&lt;style&gt;table {font-family: Calibri, sans-serif;font-size:11pt;border-collapse: collapse;width: 100%;}td, th {border: 1px solid #dddddd;text-align: left;padding:8px;}&lt;/style&gt;&lt;table&gt;&lt;tr&gt;&lt;th&gt;Date&lt;/th&gt;&lt;th&gt;Center Name&lt;/th&gt;&lt;th&gt;Center Address&lt;/th&gt;&lt;th&gt;Area&lt;/th&gt;&lt;th&gt;Pincode&lt;/th&gt;&lt;th&gt;Fee Type&lt;/th&gt;&lt;th&gt;Available Capacity&lt;/th&gt;&lt;th&gt;Vaccine Name&lt;/th&gt;&lt;th&gt;Slots Available&lt;/th&gt;&lt;/tr&gt;#DynamicTable&lt;/table&gt;&lt;br&gt;&lt;br&gt;Considering I will be busy monitoring the Cowin site for available vaccine slots, I may not be able to respond to your emails.&lt;br&gt;&lt;br&gt;To unsubscribe, please &lt;a href="#CowinExcel"&gt;click here&lt;/a&gt; and select unsubscribe from the drop down.&lt;br&gt;&lt;br&gt;Regards,&lt;br&gt;Cowin Help Bot&lt;br&gt;UiPath Professional Services-India&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>&lt;p style='font-family:Calibri;font-size:11pt'&gt;Hello,&lt;br&gt;&lt;br&gt;Hope you are safe! &lt;br&gt;&lt;br&gt;At the moment no vaccine slots are available for Pincode : &lt;b&gt;#Pincode&lt;/b&gt; and Age Limit : &lt;b&gt;#AgeLimit.&lt;/b&gt; I will keep looking for available slots and send you a notification as soon as I find one.&lt;br&gt;&lt;br&gt;Considering I will be busy monitoring the Cowin site for available vaccine slots, I may not be able to respond to your emails.&lt;br&gt;&lt;br&gt;To unsubscribe, Please  &lt;a href="#CowinExcel"&gt;click here&lt;/a&gt;  and select unsubscribe from the drop down.&lt;br&gt;&lt;br&gt;Regards,&lt;br&gt;Cowin Help Bot&lt;br&gt;UiPath Professional Services-India&lt;/p&gt;</t>
   </si>
   <si>
@@ -320,10 +314,22 @@
     <t>CowinBotEmailAddress</t>
   </si>
   <si>
-    <t>cowin-help@uipath.com</t>
-  </si>
-  <si>
     <t>C:\UiPath_Files\Cowin.xlsx</t>
+  </si>
+  <si>
+    <t>ErrorMessage_InvalidEmailAddress</t>
+  </si>
+  <si>
+    <t>The following users have entered invalid email addresses :</t>
+  </si>
+  <si>
+    <t>&lt;p style='font-family:Calibri;font-size:11pt'&gt;Hello,&lt;br&gt;&lt;br&gt;Hope you are safe! &lt;br&gt;&lt;br&gt;Please find below the list of Covid19 vaccination centers available for District : &lt;b&gt;#District&lt;/b&gt; and Age Limit : &lt;b&gt;#AgeLimit.&lt;/b&gt; Please login to &lt;a href="https://www.cowin.gov.in/home"&gt;Cowin Portal&lt;/a&gt; and block your slots immediately.&lt;br&gt;&lt;br&gt;&lt;style&gt;table {font-family: Calibri, sans-serif;font-size:11pt;border-collapse: collapse;width: 100%;}td, th {border: 1px solid #dddddd;text-align: left;padding:8px;}&lt;/style&gt;&lt;table&gt;&lt;tr&gt;&lt;th&gt;Date&lt;/th&gt;&lt;th&gt;Center Name&lt;/th&gt;&lt;th&gt;Center Address&lt;/th&gt;&lt;th&gt;Area&lt;/th&gt;&lt;th&gt;Pincode&lt;/th&gt;&lt;th&gt;Fee Type&lt;/th&gt;&lt;th&gt;Available Capacity&lt;/th&gt;&lt;th&gt;Dose1 Capacity&lt;/th&gt;&lt;th&gt;Dose2 Capacity&lt;/th&gt;&lt;th&gt;Vaccine Name&lt;/th&gt;&lt;th&gt;Slots Available&lt;/th&gt;&lt;/tr&gt;#DynamicTable&lt;/table&gt;&lt;br&gt;&lt;br&gt;Considering I will be busy monitoring the Cowin site for available vaccine slots, I may not be able to respond to your emails.&lt;br&gt;&lt;br&gt;To unsubscribe, please &lt;a href="#CowinExcel"&gt;click here&lt;/a&gt; and select unsubscribe from the drop down.&lt;br&gt;&lt;br&gt;Regards,&lt;br&gt;Cowin Help Bot&lt;br&gt;UiPath Professional Services-India&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p style='font-family:Calibri;font-size:11pt'&gt;Hello,&lt;br&gt;&lt;br&gt;Hope you are safe! &lt;br&gt;&lt;br&gt;Please find below the list of Covid19 vaccination centers available for Pincode : &lt;b&gt;#Pincode&lt;/b&gt; and Age Limit : &lt;b&gt;#AgeLimit.&lt;/b&gt; Please login to &lt;a href="https://www.cowin.gov.in/home"&gt;Cowin Portal&lt;/a&gt; and block your slots immediately.&lt;br&gt;&lt;br&gt;&lt;style&gt;table {font-family: Calibri, sans-serif;font-size:11pt;border-collapse: collapse;width: 100%;}td, th {border: 1px solid #dddddd;text-align: left;padding:8px;}&lt;/style&gt;&lt;table&gt;&lt;tr&gt;&lt;th&gt;Date&lt;/th&gt;&lt;th&gt;Center Name&lt;/th&gt;&lt;th&gt;Center Address&lt;/th&gt;&lt;th&gt;Area&lt;/th&gt;&lt;th&gt;Pincode&lt;/th&gt;&lt;th&gt;Fee Type&lt;/th&gt;&lt;th&gt;Available Capacity&lt;/th&gt;&lt;th&gt;Dose1 Capacity&lt;/th&gt;&lt;th&gt;Dose2 Capacity&lt;/th&gt;&lt;th&gt;Vaccine Name&lt;/th&gt;&lt;th&gt;Slots Available&lt;/th&gt;&lt;/tr&gt;#DynamicTable&lt;/table&gt;&lt;br&gt;&lt;br&gt;Considering I will be busy monitoring the Cowin site for available vaccine slots, I may not be able to respond to your emails.&lt;br&gt;&lt;br&gt;To unsubscribe, please &lt;a href="#CowinExcel"&gt;click here&lt;/a&gt; and select unsubscribe from the drop down.&lt;br&gt;&lt;br&gt;Regards,&lt;br&gt;Cowin Help Bot&lt;br&gt;UiPath Professional Services-India&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>sukannya.jamadar@uipath.com</t>
   </si>
 </sst>
 </file>
@@ -672,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB0D6F91-1792-4E57-8A7C-3F71DC554033}">
-  <dimension ref="A1:Z980"/>
+  <dimension ref="A1:Z981"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -689,16 +695,16 @@
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>8</v>
-      </c>
       <c r="C1" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
@@ -725,209 +731,216 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" t="s">
         <v>64</v>
-      </c>
-      <c r="B3" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" t="s">
         <v>62</v>
-      </c>
-      <c r="B6" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" t="s">
-        <v>95</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" t="s">
-        <v>51</v>
-      </c>
-    </row>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11">
-        <v>2000</v>
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>92</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" t="s">
-        <v>21</v>
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <v>2000</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
         <v>42</v>
       </c>
       <c r="D14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
-        <v>54</v>
+        <v>41</v>
+      </c>
+      <c r="D15" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" t="s">
         <v>55</v>
       </c>
-      <c r="B16" t="s">
-        <v>57</v>
-      </c>
-      <c r="C16" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>89</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="B20">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>91</v>
       </c>
-      <c r="B18">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>92</v>
-      </c>
-      <c r="B19">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>93</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="B21" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1876,10 +1889,11 @@
     <row r="978" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="979" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="980" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="981" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B20" r:id="rId1" xr:uid="{42309178-BFFA-4BD3-A87E-CB698F962D40}"/>
-    <hyperlink ref="B13" r:id="rId2" xr:uid="{34B2AEE8-3DFE-4DA1-9C69-09FED047AC7F}"/>
+    <hyperlink ref="B21" r:id="rId1" xr:uid="{42309178-BFFA-4BD3-A87E-CB698F962D40}"/>
+    <hyperlink ref="B14" r:id="rId2" xr:uid="{34B2AEE8-3DFE-4DA1-9C69-09FED047AC7F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -1904,16 +1918,16 @@
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
@@ -1940,114 +1954,114 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
         <v>30</v>
-      </c>
-      <c r="B5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
         <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
         <v>70</v>
-      </c>
-      <c r="B9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" t="s">
-        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2061,7 +2075,7 @@
   <dimension ref="A1:Y12"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2084,13 +2098,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
@@ -2117,19 +2131,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>6</v>
+        <v>95</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:25" ht="43.2" x14ac:dyDescent="0.3">
@@ -2143,13 +2157,13 @@
         <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="86.4" x14ac:dyDescent="0.3">
@@ -2157,19 +2171,19 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="43.2" x14ac:dyDescent="0.3">
@@ -2177,19 +2191,19 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="28.8" x14ac:dyDescent="0.3">
@@ -2197,16 +2211,16 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
         <v>37</v>
       </c>
-      <c r="C6" t="s">
-        <v>38</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="28.8" x14ac:dyDescent="0.3">
@@ -2214,16 +2228,16 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" t="s">
         <v>58</v>
       </c>
-      <c r="C7" t="s">
-        <v>59</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="28.8" x14ac:dyDescent="0.3">
@@ -2231,13 +2245,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="C8" t="s">
-        <v>74</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated config keys and added Annotation
</commit_message>
<xml_diff>
--- a/CowinVaccineAvailabilityProcess/Data/Config.xlsx
+++ b/CowinVaccineAvailabilityProcess/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Uipath\CowinHelpBot\CowinVaccineAvailabilityProcess\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D3E2A9-C2D0-4305-B0B7-646D9E9B3BE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E99C3402-50F7-4FCF-BFCB-631F2181D77B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -329,14 +329,14 @@
     <t>&lt;p style='font-family:Calibri;font-size:11pt'&gt;Hello,&lt;br&gt;&lt;br&gt;Hope you are safe! &lt;br&gt;&lt;br&gt;Please find below the list of Covid19 vaccination centers available for Pincode : &lt;b&gt;#Pincode&lt;/b&gt; and Age Limit : &lt;b&gt;#AgeLimit.&lt;/b&gt; Please login to &lt;a href="https://www.cowin.gov.in/home"&gt;Cowin Portal&lt;/a&gt; and block your slots immediately.&lt;br&gt;&lt;br&gt;&lt;style&gt;table {font-family: Calibri, sans-serif;font-size:11pt;border-collapse: collapse;width: 100%;}td, th {border: 1px solid #dddddd;text-align: left;padding:8px;}&lt;/style&gt;&lt;table&gt;&lt;tr&gt;&lt;th&gt;Date&lt;/th&gt;&lt;th&gt;Center Name&lt;/th&gt;&lt;th&gt;Center Address&lt;/th&gt;&lt;th&gt;Area&lt;/th&gt;&lt;th&gt;Pincode&lt;/th&gt;&lt;th&gt;Fee Type&lt;/th&gt;&lt;th&gt;Available Capacity&lt;/th&gt;&lt;th&gt;Dose1 Capacity&lt;/th&gt;&lt;th&gt;Dose2 Capacity&lt;/th&gt;&lt;th&gt;Vaccine Name&lt;/th&gt;&lt;th&gt;Slots Available&lt;/th&gt;&lt;/tr&gt;#DynamicTable&lt;/table&gt;&lt;br&gt;&lt;br&gt;Considering I will be busy monitoring the Cowin site for available vaccine slots, I may not be able to respond to your emails.&lt;br&gt;&lt;br&gt;To unsubscribe, please &lt;a href="#CowinExcel"&gt;click here&lt;/a&gt; and select unsubscribe from the drop down.&lt;br&gt;&lt;br&gt;Regards,&lt;br&gt;Cowin Help Bot&lt;br&gt;UiPath Professional Services-India&lt;/p&gt;</t>
   </si>
   <si>
-    <t>sukannya.jamadar@uipath.com</t>
+    <t>cowin-help@uipath.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -349,14 +349,6 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -382,11 +374,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -396,10 +387,8 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -681,7 +670,7 @@
   <dimension ref="A1:Z981"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -926,7 +915,7 @@
       <c r="A21" t="s">
         <v>91</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" t="s">
         <v>97</v>
       </c>
     </row>

</xml_diff>